<commit_message>
CODE IS FINISHED, might be some bugs left unsolved
</commit_message>
<xml_diff>
--- a/itemlist.xlsx
+++ b/itemlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\SCHOOL\DLSU\Term 2\PROLOGI - Programming Logic and design lecture\Project\Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8973C6E-E3E1-4133-9DF1-D5E720126731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EACF4F2-87B3-4138-BFB5-054A5CC251C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="-12" windowWidth="11112" windowHeight="8928" tabRatio="562" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="0" windowWidth="11112" windowHeight="8928" tabRatio="562" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t xml:space="preserve">sample 1 </t>
-  </si>
-  <si>
     <t>sample 4</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>chu 20</t>
+  </si>
+  <si>
+    <t>RTX 4090</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,287 +506,287 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>110000</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>323</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>2324</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>52524</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>34324</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>455</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>1000</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>300</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>400</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>450</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
         <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>